<commit_message>
Ajuste de escaleta mat 9 tema 13
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion13/ESCALETA_ MA_09_13_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion13/ESCALETA_ MA_09_13_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion13\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="7920"/>
   </bookViews>
@@ -1005,22 +1010,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1045,6 +1038,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1108,7 +1113,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1143,7 +1148,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1355,9 +1360,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U23" sqref="U23"/>
+      <selection pane="bottomLeft" activeCell="J256" sqref="J256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1386,96 +1391,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="56" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="48" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="T1" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="58" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="56"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="36" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="49"/>
-    </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="58"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>15</v>
       </c>
@@ -1878,7 +1883,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>15</v>
       </c>
@@ -2670,7 +2675,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>15</v>
       </c>
@@ -2845,7 +2850,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>15</v>
       </c>
@@ -2890,7 +2895,7 @@
       <c r="T27" s="40"/>
       <c r="U27" s="41"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>15</v>
       </c>
@@ -5607,7 +5612,7 @@
       <c r="T253" s="46"/>
       <c r="U253" s="46"/>
     </row>
-    <row r="254" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="7:21" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G254" s="30"/>
       <c r="P254" s="31"/>
       <c r="Q254" s="15"/>
@@ -5616,7 +5621,7 @@
       <c r="T254" s="46"/>
       <c r="U254" s="46"/>
     </row>
-    <row r="255" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="7:21" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G255" s="30"/>
       <c r="P255" s="31"/>
       <c r="Q255" s="15"/>
@@ -5625,7 +5630,7 @@
       <c r="T255" s="46"/>
       <c r="U255" s="46"/>
     </row>
-    <row r="256" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="7:21" s="22" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G256" s="30"/>
       <c r="P256" s="31"/>
       <c r="Q256" s="15"/>
@@ -5634,7 +5639,7 @@
       <c r="T256" s="46"/>
       <c r="U256" s="46"/>
     </row>
-    <row r="257" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="7:21" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G257" s="30"/>
       <c r="P257" s="31"/>
       <c r="Q257" s="15"/>
@@ -5643,7 +5648,7 @@
       <c r="T257" s="46"/>
       <c r="U257" s="46"/>
     </row>
-    <row r="258" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="7:21" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G258" s="30"/>
       <c r="P258" s="31"/>
       <c r="Q258" s="15"/>
@@ -5652,7 +5657,7 @@
       <c r="T258" s="46"/>
       <c r="U258" s="46"/>
     </row>
-    <row r="259" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="7:21" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G259" s="30"/>
       <c r="P259" s="31"/>
       <c r="Q259" s="15"/>
@@ -5661,7 +5666,7 @@
       <c r="T259" s="46"/>
       <c r="U259" s="46"/>
     </row>
-    <row r="260" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="7:21" s="22" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G260" s="30"/>
       <c r="P260" s="31"/>
       <c r="Q260" s="15"/>
@@ -5670,7 +5675,7 @@
       <c r="T260" s="46"/>
       <c r="U260" s="46"/>
     </row>
-    <row r="261" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="7:21" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G261" s="30"/>
       <c r="P261" s="31"/>
       <c r="Q261" s="15"/>
@@ -5679,7 +5684,7 @@
       <c r="T261" s="46"/>
       <c r="U261" s="46"/>
     </row>
-    <row r="262" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="7:21" s="22" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G262" s="30"/>
       <c r="P262" s="31"/>
       <c r="Q262" s="15"/>
@@ -5688,7 +5693,7 @@
       <c r="T262" s="46"/>
       <c r="U262" s="46"/>
     </row>
-    <row r="263" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="7:21" s="22" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G263" s="30"/>
       <c r="P263" s="31"/>
       <c r="Q263" s="15"/>
@@ -5697,7 +5702,7 @@
       <c r="T263" s="46"/>
       <c r="U263" s="46"/>
     </row>
-    <row r="264" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="7:21" s="22" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G264" s="30"/>
       <c r="P264" s="31"/>
       <c r="Q264" s="15"/>
@@ -5706,7 +5711,7 @@
       <c r="T264" s="46"/>
       <c r="U264" s="46"/>
     </row>
-    <row r="265" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="7:21" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G265" s="30"/>
       <c r="P265" s="31"/>
       <c r="Q265" s="15"/>
@@ -5715,7 +5720,7 @@
       <c r="T265" s="46"/>
       <c r="U265" s="46"/>
     </row>
-    <row r="266" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="7:21" s="22" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G266" s="30"/>
       <c r="P266" s="31"/>
       <c r="Q266" s="15"/>
@@ -5724,7 +5729,7 @@
       <c r="T266" s="46"/>
       <c r="U266" s="46"/>
     </row>
-    <row r="267" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="7:21" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G267" s="30"/>
       <c r="P267" s="31"/>
       <c r="Q267" s="15"/>
@@ -5733,7 +5738,7 @@
       <c r="T267" s="46"/>
       <c r="U267" s="46"/>
     </row>
-    <row r="268" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="7:21" s="22" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G268" s="30"/>
       <c r="P268" s="31"/>
       <c r="Q268" s="15"/>
@@ -5742,7 +5747,7 @@
       <c r="T268" s="46"/>
       <c r="U268" s="46"/>
     </row>
-    <row r="269" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="7:21" s="22" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G269" s="30"/>
       <c r="P269" s="31"/>
       <c r="Q269" s="15"/>
@@ -5751,7 +5756,7 @@
       <c r="T269" s="46"/>
       <c r="U269" s="46"/>
     </row>
-    <row r="270" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="7:21" s="22" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G270" s="30"/>
       <c r="P270" s="31"/>
       <c r="Q270" s="15"/>
@@ -5760,7 +5765,7 @@
       <c r="T270" s="46"/>
       <c r="U270" s="46"/>
     </row>
-    <row r="271" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="7:21" s="22" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G271" s="30"/>
       <c r="P271" s="31"/>
       <c r="Q271" s="15"/>
@@ -5769,7 +5774,7 @@
       <c r="T271" s="46"/>
       <c r="U271" s="46"/>
     </row>
-    <row r="272" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="7:21" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G272" s="30"/>
       <c r="P272" s="31"/>
       <c r="Q272" s="15"/>
@@ -5778,7 +5783,7 @@
       <c r="T272" s="46"/>
       <c r="U272" s="46"/>
     </row>
-    <row r="273" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="7:21" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G273" s="30"/>
       <c r="P273" s="31"/>
       <c r="Q273" s="15"/>
@@ -5787,7 +5792,7 @@
       <c r="T273" s="46"/>
       <c r="U273" s="46"/>
     </row>
-    <row r="274" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="7:21" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G274" s="30"/>
       <c r="P274" s="31"/>
       <c r="Q274" s="15"/>
@@ -5796,7 +5801,7 @@
       <c r="T274" s="46"/>
       <c r="U274" s="46"/>
     </row>
-    <row r="275" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="7:21" s="22" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G275" s="30"/>
       <c r="P275" s="31"/>
       <c r="Q275" s="15"/>
@@ -5805,7 +5810,7 @@
       <c r="T275" s="46"/>
       <c r="U275" s="46"/>
     </row>
-    <row r="276" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="7:21" s="22" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G276" s="30"/>
       <c r="P276" s="31"/>
       <c r="Q276" s="15"/>
@@ -5814,7 +5819,7 @@
       <c r="T276" s="46"/>
       <c r="U276" s="46"/>
     </row>
-    <row r="277" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="7:21" s="22" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G277" s="30"/>
       <c r="P277" s="31"/>
       <c r="Q277" s="15"/>
@@ -5823,7 +5828,7 @@
       <c r="T277" s="46"/>
       <c r="U277" s="46"/>
     </row>
-    <row r="278" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="7:21" s="22" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G278" s="30"/>
       <c r="P278" s="31"/>
       <c r="Q278" s="15"/>
@@ -5832,7 +5837,7 @@
       <c r="T278" s="46"/>
       <c r="U278" s="46"/>
     </row>
-    <row r="279" spans="7:21" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="7:21" s="22" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G279" s="30"/>
       <c r="P279" s="31"/>
       <c r="Q279" s="15"/>
@@ -5850,6 +5855,12 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5864,12 +5875,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>